<commit_message>
commit code export file excel with poi lib
</commit_message>
<xml_diff>
--- a/src/data.xlsx
+++ b/src/data.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ViHuan-Mentor-FU\FU-OOP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37585A0F-514E-41C1-8909-5AB537EFF718}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D75A72F6-A792-4A4C-865B-C0FA8BBA8673}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8970" yWindow="45" windowWidth="19695" windowHeight="15495" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="results" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="5">
   <si>
     <t>start_type</t>
   </si>
@@ -43,20 +43,13 @@
     <t>Vowel</t>
   </si>
   <si>
-    <t>Consonant</t>
-  </si>
-  <si>
     <t>id</t>
-  </si>
-  <si>
-    <t>huanvc30</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -891,351 +884,71 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="29.7109375"/>
+    <col min="2" max="2" width="29.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s" s="0">
-        <v>5</v>
-      </c>
-      <c r="B1" t="s" s="0">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s" s="0">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s" s="0">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="0">
+      <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="0">
+      <c r="C2">
         <v>80</v>
       </c>
-      <c r="D2" s="0">
+      <c r="D2">
         <v>22.792022790000001</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="0">
+      <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="s" s="0">
-        <v>4</v>
-      </c>
-      <c r="C3" s="0">
-        <v>271</v>
-      </c>
-      <c r="D3" s="0">
-        <v>77.207977209999996</v>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>80</v>
+      </c>
+      <c r="D3">
+        <v>22.792022790000001</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="0">
+      <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" t="s" s="0">
+      <c r="B4" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="0">
+      <c r="C4">
         <v>80</v>
       </c>
-      <c r="D4" s="0">
+      <c r="D4">
         <v>22.792022790000001</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="0">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s" s="0">
-        <v>4</v>
-      </c>
-      <c r="C5" s="0">
-        <v>271</v>
-      </c>
-      <c r="D5" s="0">
-        <v>77.207977209999996</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="0">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s" s="0">
-        <v>3</v>
-      </c>
-      <c r="C6" s="0">
-        <v>80</v>
-      </c>
-      <c r="D6" s="0">
-        <v>22.792022790000001</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="0">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s" s="0">
-        <v>4</v>
-      </c>
-      <c r="C7" s="0">
-        <v>271</v>
-      </c>
-      <c r="D7" s="0">
-        <v>77.207977209999996</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="0">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s" s="0">
-        <v>3</v>
-      </c>
-      <c r="C8" s="0">
-        <v>80</v>
-      </c>
-      <c r="D8" s="0">
-        <v>22.792022790000001</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="0">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s" s="0">
-        <v>4</v>
-      </c>
-      <c r="C9" s="0">
-        <v>271</v>
-      </c>
-      <c r="D9" s="0">
-        <v>77.207977209999996</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="0">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s" s="0">
-        <v>3</v>
-      </c>
-      <c r="C10" s="0">
-        <v>80</v>
-      </c>
-      <c r="D10" s="0">
-        <v>22.792022790000001</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="0">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s" s="0">
-        <v>4</v>
-      </c>
-      <c r="C11" s="0">
-        <v>271</v>
-      </c>
-      <c r="D11" s="0">
-        <v>77.207977209999996</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="0">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s" s="0">
-        <v>3</v>
-      </c>
-      <c r="C12" s="0">
-        <v>80</v>
-      </c>
-      <c r="D12" s="0">
-        <v>22.792022790000001</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="0">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s" s="0">
-        <v>4</v>
-      </c>
-      <c r="C13" s="0">
-        <v>271</v>
-      </c>
-      <c r="D13" s="0">
-        <v>77.207977209999996</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="0">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s" s="0">
-        <v>3</v>
-      </c>
-      <c r="C14" s="0">
-        <v>80</v>
-      </c>
-      <c r="D14" s="0">
-        <v>22.792022790000001</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="0">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s" s="0">
-        <v>4</v>
-      </c>
-      <c r="C15" s="0">
-        <v>271</v>
-      </c>
-      <c r="D15" s="0">
-        <v>77.207977209999996</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="0">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s" s="0">
-        <v>3</v>
-      </c>
-      <c r="C16" s="0">
-        <v>80</v>
-      </c>
-      <c r="D16" s="0">
-        <v>22.792022790000001</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="0">
-        <v>16</v>
-      </c>
-      <c r="B17" t="s" s="0">
-        <v>4</v>
-      </c>
-      <c r="C17" s="0">
-        <v>271</v>
-      </c>
-      <c r="D17" s="0">
-        <v>77.207977209999996</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="0">
-        <v>17</v>
-      </c>
-      <c r="B18" t="s" s="0">
-        <v>3</v>
-      </c>
-      <c r="C18" s="0">
-        <v>80</v>
-      </c>
-      <c r="D18" s="0">
-        <v>22.792022790000001</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="0">
-        <v>18</v>
-      </c>
-      <c r="B19" t="s" s="0">
-        <v>4</v>
-      </c>
-      <c r="C19" s="0">
-        <v>271</v>
-      </c>
-      <c r="D19" s="0">
-        <v>77.207977209999996</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="0">
-        <v>19</v>
-      </c>
-      <c r="B20" t="s" s="0">
-        <v>3</v>
-      </c>
-      <c r="C20" s="0">
-        <v>80</v>
-      </c>
-      <c r="D20" s="0">
-        <v>22.792022790000001</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="0">
-        <v>20</v>
-      </c>
-      <c r="B21" t="s" s="0">
-        <v>4</v>
-      </c>
-      <c r="C21" s="0">
-        <v>271</v>
-      </c>
-      <c r="D21" s="0">
-        <v>77.207977209999996</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="0">
-        <v>21</v>
-      </c>
-      <c r="B22" t="s" s="0">
-        <v>3</v>
-      </c>
-      <c r="C22" s="0">
-        <v>80</v>
-      </c>
-      <c r="D22" s="0">
-        <v>22.792022790000001</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="0">
-        <v>22</v>
-      </c>
-      <c r="B23" t="s" s="0">
-        <v>4</v>
-      </c>
-      <c r="C23" s="0">
-        <v>271</v>
-      </c>
-      <c r="D23" s="0">
-        <v>77.207977209999996</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="n" s="0">
-        <v>30.0</v>
-      </c>
-      <c r="B24" t="s" s="0">
-        <v>6</v>
-      </c>
-      <c r="C24" t="n" s="0">
-        <v>23.0</v>
-      </c>
-      <c r="D24" t="n" s="0">
-        <v>22.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>